<commit_message>
Updated results (removed duplicates)
</commit_message>
<xml_diff>
--- a/Query_CSVs/Final_Excel.xlsx
+++ b/Query_CSVs/Final_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aashu\AashuCoursework\Projects\IBM\Queries_Responses\Query_CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14DA640-6E54-4CE0-93F0-ED042C387D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BF7EEA-D9AD-4B3C-B8CC-FB8FF5BCA511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D965821-77E7-49C0-9D68-8485EF54A075}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D965821-77E7-49C0-9D68-8485EF54A075}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,8 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,28 +550,28 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I2">
-        <v>295</v>
+        <v>40</v>
       </c>
       <c r="J2">
-        <v>81</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -587,7 +588,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3">
         <v>13</v>
@@ -596,10 +597,10 @@
         <v>6</v>
       </c>
       <c r="H3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3">
         <v>23</v>
@@ -616,25 +617,25 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I4">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="J4">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -651,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -660,10 +661,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -677,13 +678,13 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <v>12</v>
@@ -695,7 +696,7 @@
         <v>27</v>
       </c>
       <c r="I6">
-        <v>690</v>
+        <v>658</v>
       </c>
       <c r="J6">
         <v>80</v>
@@ -718,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -727,10 +728,10 @@
         <v>5</v>
       </c>
       <c r="I7">
-        <v>227</v>
+        <v>42</v>
       </c>
       <c r="J7">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -759,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -791,10 +792,10 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>